<commit_message>
Day04(SQL table modified) Week07/Day01(Spring Enviroment created//HelloController created to exercise one)
</commit_message>
<xml_diff>
--- a/Week-06/Day04/SQL.xlsx
+++ b/Week-06/Day04/SQL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
   <si>
     <t>SELECT</t>
   </si>
@@ -1424,18 +1424,38 @@
   </si>
   <si>
     <t>To avoid null values in a coloumn</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>SELECT col_expression AS expr_description</t>
+  </si>
+  <si>
+    <t>if your select method made more complex with basic arithmetical operations (or with anything else) you'd better describe it right after it with an alias</t>
+  </si>
+  <si>
+    <t>every columns and tables could have alias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1657,13 +1677,10 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1672,63 +1689,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2062,373 +2082,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="67.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="67.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C8" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="C11" s="6" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="C12" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="6" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="5" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="5" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D17" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11" t="s">
+    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D18" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="5" t="s">
+    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="11" t="s">
+    <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D20" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="33" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="11" t="s">
+    <row r="21" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D21" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E21" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="5" t="s">
+    <row r="22" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C22" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D22" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E22" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="15" t="s">
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D23" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E23" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="15" t="s">
+    <row r="24" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D24" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="23"/>
-    </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D26" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E26" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18" t="s">
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C27" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21" t="s">
+      <c r="D27" s="23"/>
+      <c r="E27" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C29" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A16:A23"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="F25:H26"/>
-    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A17:A24"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:H27"/>
+    <mergeCell ref="A10:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Week07/Day03(Enviroment created) Week06/Day04(more things added)
</commit_message>
<xml_diff>
--- a/Week-06/Day04/SQL.xlsx
+++ b/Week-06/Day04/SQL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="167">
   <si>
     <t>SELECT</t>
   </si>
@@ -1436,13 +1436,638 @@
   </si>
   <si>
     <t>every columns and tables could have alias</t>
+  </si>
+  <si>
+    <t>ROUND</t>
+  </si>
+  <si>
+    <t>ROUND (coloumn)</t>
+  </si>
+  <si>
+    <t>Rounds a float number into an integer</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>COUNT()</t>
+  </si>
+  <si>
+    <t>MIN()</t>
+  </si>
+  <si>
+    <t>MAX()</t>
+  </si>
+  <si>
+    <t>AVG()</t>
+  </si>
+  <si>
+    <t>SUM()</t>
+  </si>
+  <si>
+    <r>
+      <t>MIN(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coloumn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>COUNT(*)/(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coloumn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MAX(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coloumn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>AVG(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coloumn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SUM(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coloumn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Counts the number of rows in the group / Does the same without NULL in the specified coloumn</t>
+  </si>
+  <si>
+    <t>Finds the smallest numerical value in the specified column for all rows in the group.</t>
+  </si>
+  <si>
+    <t>Finds the largest numerical value in the specified column for all rows in the group.</t>
+  </si>
+  <si>
+    <t>Finds the average numerical value in the specified column for all rows in the group.</t>
+  </si>
+  <si>
+    <t>Finds the sum of all numerical values in the specified column for the rows in the group.</t>
+  </si>
+  <si>
+    <t>GROUP BY</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GROUP BY </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coloumn</t>
+    </r>
+  </si>
+  <si>
+    <t>Groups the given coloumn's raws if they are containing the same values specified</t>
+  </si>
+  <si>
+    <t>Given 20 raws of data of the age, and given 3 role positions, if you would like to get each role position's avarage age, then you calculate the avarage then GROUP BY the role position</t>
+  </si>
+  <si>
+    <t>HAVING</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HAVING </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>group_condition</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">For filtering after the groupping </t>
+  </si>
+  <si>
+    <t>LEFT JOIN</t>
+  </si>
+  <si>
+    <t>RIGHT JOIN</t>
+  </si>
+  <si>
+    <t>OUTTER JOIN</t>
+  </si>
+  <si>
+    <t>FULL OUTTER JOIN</t>
+  </si>
+  <si>
+    <t>INSERT</t>
+  </si>
+  <si>
+    <t>INTO</t>
+  </si>
+  <si>
+    <t>INSERT INTO myTable</t>
+  </si>
+  <si>
+    <t>(coloumn, another_coloumn)</t>
+  </si>
+  <si>
+    <t>VALUES</t>
+  </si>
+  <si>
+    <t>VALUES (value_or_expression, another, ...),</t>
+  </si>
+  <si>
+    <t>…;</t>
+  </si>
+  <si>
+    <t>(value_or_expression, another, ...),</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>UPDATE myTable</t>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <t>SET column = value_or_exp,</t>
+  </si>
+  <si>
+    <t>another column = value_or_exp2,</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updates all the rows, you can specify rows by WHERE clause. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALWAYS write the SELECT query and where clause first, then update if it selects thoose rows what you want</t>
+    </r>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>DELETE FROM myTable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WHERE </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>condition</t>
+    </r>
+  </si>
+  <si>
+    <t>Deletes the rows according to the condition</t>
+  </si>
+  <si>
+    <r>
+      <t>Deletes all the rows.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ALWAYS write the SELECT query and where clause first, then delete if it selects thoose rows what you want</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TABLE </t>
+  </si>
+  <si>
+    <t>IF NOT EXIST</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE TABLE IF NOT EXIST </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>myTable (</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">column </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DataType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TableConstraint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5D5C58"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>default_value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">another_column </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DataType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TableConstraint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5D5C58"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>default_value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>Data Types</t>
+  </si>
+  <si>
+    <t>INTEGER, BOOLEAN</t>
+  </si>
+  <si>
+    <t>FLOAT, DOUBLE, REAL</t>
+  </si>
+  <si>
+    <t>CHARACTER(num_chars), VARCHAR(num_chars), TEXT</t>
+  </si>
+  <si>
+    <t>DATE, DATATIME</t>
+  </si>
+  <si>
+    <t>BLOB</t>
+  </si>
+  <si>
+    <t>The integer datatypes can store whole integer values like the count of a number or an age. In some implementations, the boolean value is just represented as an integer value of just 0 or 1.</t>
+  </si>
+  <si>
+    <t>The floating point datatypes can store more precise numerical data like measurements or fractional values. Different types can be used depending on the floating point precision required for that value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The text based datatypes can store strings and text in all sorts of locales. The distinction between the various types generally amount to underlaying efficiency of the database when working with these columns. Both the CHARACTER and VARCHAR (variable character) types are specified with the max number of characters that they can store (longer values may be truncated), so can be more efficient to store and query with big tables</t>
+  </si>
+  <si>
+    <t>SQL can also store date and time stamps to keep track of time series and event data. They can be tricky to work with especially when manipulating data across timezones.</t>
+  </si>
+  <si>
+    <t>Finally, SQL can store binary data in blobs right in the database. These values are often opaque to the database, so you usually have to store them with the right metadata to requery them.</t>
+  </si>
+  <si>
+    <t>Table Constraints</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>AUTOINCREMENT</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>CHECK (expression)</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY</t>
+  </si>
+  <si>
+    <t>This means that the values in this column are unique, and each value can be used to identify a single row in this table.</t>
+  </si>
+  <si>
+    <t>For integer values, this means that the value is automatically filled in and incremented with each row insertion. Not supported in all databases.</t>
+  </si>
+  <si>
+    <t>This means that the values in this column have to be unique, so you can't insert another row with the same value in this column as another row in the table. Differs from the `PRIMARY KEY` in that it doesn't have to be a key for a row in the table.</t>
+  </si>
+  <si>
+    <t>This means that the inserted value can not be `NULL`.</t>
+  </si>
+  <si>
+    <t>This is allows you to run a more complex expression to test whether the values inserted are value. For example, you can check that values are positive, or greater than a specific size, or start with a certain prefix, etc.</t>
+  </si>
+  <si>
+    <t>This is a consistency check which ensures that each value in this column corresponds to another value in a column in another table. For example, if there are two tables, one listing all Employees by ID, and another listing their payroll information, the `FOREIGN KEY` can ensure that every row in the payroll table corresponds to a valid employee in the master Employee list.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1615,6 +2240,23 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF5D5C58"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1648,7 +2290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1671,11 +2313,165 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1723,18 +2519,18 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1749,6 +2545,77 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2082,22 +2949,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76:D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="67.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -2114,7 +2981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2125,7 +2992,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
@@ -2136,7 +3003,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>44</v>
       </c>
@@ -2150,7 +3017,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>85</v>
       </c>
@@ -2164,305 +3031,834 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C24" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="4" t="s">
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="C12" s="5" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
+      <c r="C28" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="6" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="B29" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="4" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="4" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+    <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D33" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="8" t="s">
+    <row r="34" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="4" t="s">
+    <row r="35" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="8" t="s">
+    <row r="36" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="33" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="8" t="s">
+    <row r="37" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+      <c r="B37" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="4" t="s">
+    <row r="38" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A38" s="22"/>
+      <c r="B38" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C38" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="11" t="s">
+    <row r="39" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22"/>
+      <c r="B39" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C39" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E39" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="11" t="s">
+    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="22"/>
+      <c r="B40" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C40" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="20"/>
-    </row>
-    <row r="25" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-    </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-    </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C43" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C50" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C51" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D53" s="27"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C54" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" s="27"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C55" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" s="28"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="29"/>
+    </row>
+    <row r="57" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D59" s="26"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C60" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D60" s="27"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C61" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D61" s="27"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C62" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D62" s="28"/>
+    </row>
+    <row r="64" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A64" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B64" s="50"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
+      <c r="J64" s="31"/>
+      <c r="K64" s="31"/>
+    </row>
+    <row r="65" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="31"/>
+      <c r="K65" s="31"/>
+    </row>
+    <row r="66" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="31"/>
+      <c r="H66" s="31"/>
+      <c r="I66" s="31"/>
+      <c r="J66" s="31"/>
+      <c r="K66" s="31"/>
+    </row>
+    <row r="67" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="C67" s="34"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="31"/>
+      <c r="K67" s="31"/>
+    </row>
+    <row r="68" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
+      <c r="H68" s="31"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="31"/>
+      <c r="K68" s="31"/>
+    </row>
+    <row r="69" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="B69" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="31"/>
+      <c r="H69" s="31"/>
+      <c r="I69" s="31"/>
+      <c r="J69" s="31"/>
+      <c r="K69" s="31"/>
+    </row>
+    <row r="71" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A71" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" s="50"/>
+      <c r="C71" s="50"/>
+      <c r="D71" s="50"/>
+    </row>
+    <row r="72" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B72" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="42"/>
+      <c r="D72" s="43"/>
+      <c r="E72" s="33"/>
+    </row>
+    <row r="73" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C73" s="38"/>
+      <c r="D73" s="39"/>
+    </row>
+    <row r="74" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="38"/>
+      <c r="D74" s="39"/>
+    </row>
+    <row r="75" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B75" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" s="38"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="33"/>
+    </row>
+    <row r="76" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B76" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C76" s="45"/>
+      <c r="D76" s="46"/>
+      <c r="E76" s="33"/>
+    </row>
+    <row r="77" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B77" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="C77" s="48"/>
+      <c r="D77" s="49"/>
+      <c r="E77" s="33"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="40"/>
+      <c r="C78" s="40"/>
+      <c r="D78" s="40"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A17:A24"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="F26:H27"/>
-    <mergeCell ref="A10:A16"/>
+  <mergeCells count="20">
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:H15"/>
+    <mergeCell ref="A26:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>